<commit_message>
tech and regional aspect added
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\hravoaha\Desktop\Thèse\process-development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B688038-4A8C-463B-A919-63657C32E538}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CCFC1F0-558B-439B-8D28-DBA481FC285E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" firstSheet="1" activeTab="4" xr2:uid="{14B8D0C9-091E-43B5-9C59-8A05020574F1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" firstSheet="1" activeTab="6" xr2:uid="{14B8D0C9-091E-43B5-9C59-8A05020574F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Composition of waste" sheetId="4" r:id="rId1"/>
-    <sheet name="Variables" sheetId="1" r:id="rId2"/>
-    <sheet name="Composition (mass)" sheetId="6" r:id="rId3"/>
+    <sheet name="Composition (mass)" sheetId="6" r:id="rId2"/>
+    <sheet name="Variables" sheetId="1" r:id="rId3"/>
     <sheet name="stoe" sheetId="7" r:id="rId4"/>
     <sheet name="kinetics" sheetId="2" r:id="rId5"/>
-    <sheet name="Paramètres d'opérations" sheetId="3" r:id="rId6"/>
+    <sheet name="tech" sheetId="3" r:id="rId6"/>
+    <sheet name="reg" sheetId="8" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Composition (mass)'!$B$1:$B$97</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Composition (mass)'!$B$1:$B$97</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Composition of waste'!$B$1:$B$113</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="423">
   <si>
     <t>Variables</t>
   </si>
@@ -1245,31 +1246,7 @@
     <t>Ammonium saturation constant</t>
   </si>
   <si>
-    <t>Qair</t>
-  </si>
-  <si>
-    <t>Débit d'air entrant</t>
-  </si>
-  <si>
-    <t>kg air.h-1</t>
-  </si>
-  <si>
-    <t>Aéré passivement (par retournement)</t>
-  </si>
-  <si>
-    <t>Aéré par soufflement d'air à l'air libre</t>
-  </si>
-  <si>
-    <t>Aéré par soufflement d'air dans un contenant</t>
-  </si>
-  <si>
     <t>Temperature of the pile</t>
-  </si>
-  <si>
-    <t>Free convection</t>
-  </si>
-  <si>
-    <t>Forced convection</t>
   </si>
   <si>
     <t>mass</t>
@@ -1291,6 +1268,42 @@
   </si>
   <si>
     <t>khS</t>
+  </si>
+  <si>
+    <t>Ta</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>IC</t>
+  </si>
+  <si>
+    <t>Unity</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Heat transfer coefficient of wall</t>
+  </si>
+  <si>
+    <t>kJ/m2.°C.h</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>surface area of heat conduction</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>hc</t>
+  </si>
+  <si>
+    <t>GLO</t>
   </si>
 </sst>
 </file>
@@ -25075,898 +25088,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A13E0657-BE6C-45BC-B891-D54361BD0D37}">
-  <dimension ref="A1:M37"/>
-  <sheetViews>
-    <sheetView zoomScale="84" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="7.08984375" customWidth="1"/>
-    <col min="2" max="2" width="12.81640625" customWidth="1"/>
-    <col min="3" max="3" width="10.90625" customWidth="1"/>
-    <col min="4" max="4" width="24.453125" customWidth="1"/>
-    <col min="5" max="11" width="10.90625" customWidth="1"/>
-    <col min="12" max="12" width="13.54296875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="B2" s="2">
-        <f>'Composition (mass)'!BR97</f>
-        <v>9.6732052453432296</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="F2">
-        <v>6</v>
-      </c>
-      <c r="G2">
-        <v>12</v>
-      </c>
-      <c r="H2">
-        <v>6</v>
-      </c>
-      <c r="L2">
-        <f>($F2*12)+($G2*1)+($H2*16)+($I2*14)</f>
-        <v>180</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2">
-        <f>'Composition (mass)'!BO97</f>
-        <v>1.4155222050567735</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="F3">
-        <v>16</v>
-      </c>
-      <c r="G3">
-        <v>24</v>
-      </c>
-      <c r="H3">
-        <v>5</v>
-      </c>
-      <c r="I3">
-        <v>4</v>
-      </c>
-      <c r="L3">
-        <f t="shared" ref="L3:L21" si="0">($F3*12)+($G3*1)+($H3*16)+($I3*14)</f>
-        <v>352</v>
-      </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2">
-        <f>'Composition (mass)'!BP97</f>
-        <v>1.4893321688918979</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="F4">
-        <v>25</v>
-      </c>
-      <c r="G4">
-        <v>45</v>
-      </c>
-      <c r="H4">
-        <v>3</v>
-      </c>
-      <c r="L4">
-        <f t="shared" si="0"/>
-        <v>393</v>
-      </c>
-      <c r="M4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="B5" s="2">
-        <f>'Composition (mass)'!BL97</f>
-        <v>0</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="F5">
-        <v>10</v>
-      </c>
-      <c r="G5">
-        <v>18</v>
-      </c>
-      <c r="H5">
-        <v>9</v>
-      </c>
-      <c r="L5">
-        <f t="shared" si="0"/>
-        <v>282</v>
-      </c>
-      <c r="M5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="2">
-        <f>'Composition (mass)'!BK97</f>
-        <v>1.1647929815279715E-2</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="2">
-        <f>'Composition (mass)'!BN97</f>
-        <v>6.8117678833062613E-3</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="F7">
-        <v>20</v>
-      </c>
-      <c r="G7">
-        <v>30</v>
-      </c>
-      <c r="H7">
-        <v>6</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="0"/>
-        <v>366</v>
-      </c>
-      <c r="M7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="B8" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="F9">
-        <v>6</v>
-      </c>
-      <c r="G9">
-        <v>12</v>
-      </c>
-      <c r="H9">
-        <v>6</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="0"/>
-        <v>180</v>
-      </c>
-      <c r="M9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="F10">
-        <v>16</v>
-      </c>
-      <c r="G10">
-        <v>24</v>
-      </c>
-      <c r="H10">
-        <v>5</v>
-      </c>
-      <c r="I10">
-        <v>4</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="0"/>
-        <v>352</v>
-      </c>
-      <c r="M10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="2">
-        <v>0</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="F11">
-        <v>25</v>
-      </c>
-      <c r="G11">
-        <v>45</v>
-      </c>
-      <c r="H11">
-        <v>3</v>
-      </c>
-      <c r="L11">
-        <f t="shared" si="0"/>
-        <v>393</v>
-      </c>
-      <c r="M11">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="2">
-        <v>0</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="F12">
-        <v>10</v>
-      </c>
-      <c r="G12">
-        <v>18</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="0"/>
-        <v>138</v>
-      </c>
-      <c r="M12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="2">
-        <v>0</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="F13">
-        <v>20</v>
-      </c>
-      <c r="G13">
-        <v>30</v>
-      </c>
-      <c r="H13">
-        <v>6</v>
-      </c>
-      <c r="L13">
-        <f t="shared" si="0"/>
-        <v>366</v>
-      </c>
-      <c r="M13">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14">
-        <v>0.1</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="F14">
-        <v>5</v>
-      </c>
-      <c r="G14">
-        <v>7</v>
-      </c>
-      <c r="H14">
-        <v>2</v>
-      </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="0"/>
-        <v>113</v>
-      </c>
-      <c r="M14">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15">
-        <v>0.1</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="F15">
-        <v>5</v>
-      </c>
-      <c r="G15">
-        <v>7</v>
-      </c>
-      <c r="H15">
-        <v>2</v>
-      </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="L15">
-        <f t="shared" si="0"/>
-        <v>113</v>
-      </c>
-      <c r="M15">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16">
-        <v>0.1</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="F16">
-        <v>5</v>
-      </c>
-      <c r="G16">
-        <v>7</v>
-      </c>
-      <c r="H16">
-        <v>2</v>
-      </c>
-      <c r="I16">
-        <v>1</v>
-      </c>
-      <c r="L16">
-        <f t="shared" si="0"/>
-        <v>113</v>
-      </c>
-      <c r="M16">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17">
-        <v>0.1</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="F17">
-        <v>5</v>
-      </c>
-      <c r="G17">
-        <v>7</v>
-      </c>
-      <c r="H17">
-        <v>2</v>
-      </c>
-      <c r="I17">
-        <v>1</v>
-      </c>
-      <c r="L17">
-        <f t="shared" si="0"/>
-        <v>113</v>
-      </c>
-      <c r="M17">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18">
-        <v>0.1</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="F18">
-        <v>10</v>
-      </c>
-      <c r="G18">
-        <v>17</v>
-      </c>
-      <c r="H18">
-        <v>6</v>
-      </c>
-      <c r="I18">
-        <v>1</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="0"/>
-        <v>247</v>
-      </c>
-      <c r="M18">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19">
-        <v>0.1</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="F19">
-        <v>10</v>
-      </c>
-      <c r="G19">
-        <v>17</v>
-      </c>
-      <c r="H19">
-        <v>6</v>
-      </c>
-      <c r="I19">
-        <v>1</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="0"/>
-        <v>247</v>
-      </c>
-      <c r="M19">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="B20">
-        <v>0.1</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="B21">
-        <v>0.1</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="F21">
-        <v>5</v>
-      </c>
-      <c r="G21">
-        <v>7</v>
-      </c>
-      <c r="H21">
-        <v>2</v>
-      </c>
-      <c r="I21">
-        <v>1</v>
-      </c>
-      <c r="L21">
-        <f t="shared" si="0"/>
-        <v>113</v>
-      </c>
-      <c r="M21">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="B22">
-        <f>'Composition (mass)'!D97</f>
-        <v>7.1692660173160174</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L25">
-        <f>($F25*12)+($G25*1)+($H25*16)+($I25*14)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A26" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A31" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>401</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="597" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35DF1B96-6F36-403A-A03F-B41BA123E54D}">
   <dimension ref="A1:CB97"/>
   <sheetViews>
@@ -50011,6 +49132,898 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A13E0657-BE6C-45BC-B891-D54361BD0D37}">
+  <dimension ref="A1:M37"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" zoomScale="84" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="7.08984375" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" customWidth="1"/>
+    <col min="3" max="3" width="10.90625" customWidth="1"/>
+    <col min="4" max="4" width="24.453125" customWidth="1"/>
+    <col min="5" max="11" width="10.90625" customWidth="1"/>
+    <col min="12" max="12" width="13.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B2" s="2">
+        <f>'Composition (mass)'!BR97</f>
+        <v>9.6732052453432296</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <v>12</v>
+      </c>
+      <c r="H2">
+        <v>6</v>
+      </c>
+      <c r="L2">
+        <f>($F2*12)+($G2*1)+($H2*16)+($I2*14)</f>
+        <v>180</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2">
+        <f>'Composition (mass)'!BO97</f>
+        <v>1.4155222050567735</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="F3">
+        <v>16</v>
+      </c>
+      <c r="G3">
+        <v>24</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="I3">
+        <v>4</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L21" si="0">($F3*12)+($G3*1)+($H3*16)+($I3*14)</f>
+        <v>352</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2">
+        <f>'Composition (mass)'!BP97</f>
+        <v>1.4893321688918979</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="F4">
+        <v>25</v>
+      </c>
+      <c r="G4">
+        <v>45</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>393</v>
+      </c>
+      <c r="M4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B5" s="2">
+        <f>'Composition (mass)'!BL97</f>
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>18</v>
+      </c>
+      <c r="H5">
+        <v>9</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>282</v>
+      </c>
+      <c r="M5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2">
+        <f>'Composition (mass)'!BK97</f>
+        <v>1.1647929815279715E-2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2">
+        <f>'Composition (mass)'!BN97</f>
+        <v>6.8117678833062613E-3</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="F7">
+        <v>20</v>
+      </c>
+      <c r="G7">
+        <v>30</v>
+      </c>
+      <c r="H7">
+        <v>6</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>366</v>
+      </c>
+      <c r="M7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+      <c r="G9">
+        <v>12</v>
+      </c>
+      <c r="H9">
+        <v>6</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="M9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="F10">
+        <v>16</v>
+      </c>
+      <c r="G10">
+        <v>24</v>
+      </c>
+      <c r="H10">
+        <v>5</v>
+      </c>
+      <c r="I10">
+        <v>4</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>352</v>
+      </c>
+      <c r="M10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="F11">
+        <v>25</v>
+      </c>
+      <c r="G11">
+        <v>45</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>393</v>
+      </c>
+      <c r="M11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <v>18</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>138</v>
+      </c>
+      <c r="M12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="F13">
+        <v>20</v>
+      </c>
+      <c r="G13">
+        <v>30</v>
+      </c>
+      <c r="H13">
+        <v>6</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>366</v>
+      </c>
+      <c r="M13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <v>0.1</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
+      <c r="G14">
+        <v>7</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>113</v>
+      </c>
+      <c r="M14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15">
+        <v>0.1</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="F15">
+        <v>5</v>
+      </c>
+      <c r="G15">
+        <v>7</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>113</v>
+      </c>
+      <c r="M15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16">
+        <v>0.1</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="F16">
+        <v>5</v>
+      </c>
+      <c r="G16">
+        <v>7</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>113</v>
+      </c>
+      <c r="M16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17">
+        <v>0.1</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="F17">
+        <v>5</v>
+      </c>
+      <c r="G17">
+        <v>7</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>113</v>
+      </c>
+      <c r="M17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18">
+        <v>0.1</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="F18">
+        <v>10</v>
+      </c>
+      <c r="G18">
+        <v>17</v>
+      </c>
+      <c r="H18">
+        <v>6</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>247</v>
+      </c>
+      <c r="M18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19">
+        <v>0.1</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="F19">
+        <v>10</v>
+      </c>
+      <c r="G19">
+        <v>17</v>
+      </c>
+      <c r="H19">
+        <v>6</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>247</v>
+      </c>
+      <c r="M19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="B20">
+        <v>0.1</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B21">
+        <v>0.1</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="F21">
+        <v>5</v>
+      </c>
+      <c r="G21">
+        <v>7</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="0"/>
+        <v>113</v>
+      </c>
+      <c r="M21">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B22">
+        <f>'Composition (mass)'!D97</f>
+        <v>7.1692660173160174</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L25">
+        <f>($F25*12)+($G25*1)+($H25*16)+($I25*14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>401</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="597" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02BDDFCB-2B9F-4872-A820-97635CABD872}">
   <dimension ref="A1:B12"/>
@@ -50026,15 +50039,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="B1" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="B2" s="2">
         <v>0.35</v>
@@ -50123,7 +50136,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="B12" s="2">
         <v>0.2</v>
@@ -50139,16 +50152,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99E22A85-0A6D-4692-91B9-50CA4D04329A}">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="B1:D1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.6328125" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" style="23" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6328125" style="23" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="45.54296875" style="23" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.54296875" style="23" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="10.90625" style="23"/>
   </cols>
   <sheetData>
@@ -50661,7 +50674,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="B31" s="24">
         <v>1E-4</v>
@@ -50874,63 +50887,141 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68CD580C-396B-4BB3-AD93-6F2493BB33D0}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="13.1796875" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="5" max="5" width="9.453125" customWidth="1"/>
+    <col min="6" max="6" width="13.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="B2" s="2">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>410</v>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="B3" s="2">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2">
+        <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E3" s="2" t="s">
-        <v>407</v>
-      </c>
-      <c r="G3" t="s">
-        <v>411</v>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="B4" s="2">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2">
+        <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E4" s="2" t="s">
-        <v>408</v>
-      </c>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="597" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4331B1-DB9B-40DE-AC61-5ECF54032BDB}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>422</v>
+      </c>
+      <c r="B2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B3">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
temperature profile to solve
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20395"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\hravoaha\Desktop\Thèse\process-development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C992CDD-D24D-45B3-BA00-FB47E2272D52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDC96D5-7743-4E26-BC2A-147BE00AB840}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="4" xr2:uid="{14B8D0C9-091E-43B5-9C59-8A05020574F1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="5" xr2:uid="{14B8D0C9-091E-43B5-9C59-8A05020574F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Composition of waste" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="497">
   <si>
     <t>Variables</t>
   </si>
@@ -1288,9 +1288,6 @@
     <t>Heat transfer coefficient of wall</t>
   </si>
   <si>
-    <t>kJ/m2.°C.h</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -1298,9 +1295,6 @@
   </si>
   <si>
     <t>u</t>
-  </si>
-  <si>
-    <t>hc</t>
   </si>
   <si>
     <t>GLO</t>
@@ -1377,6 +1371,164 @@
   <si>
     <t>https://www.mdpi.com/1999-4907/13/6/914/htm#:~:text=The%20specific%20heat%20capacity%20of,effects%20on%20specific%20heat%20capacity.</t>
   </si>
+  <si>
+    <t>Tmax,2</t>
+  </si>
+  <si>
+    <t>Topt,2</t>
+  </si>
+  <si>
+    <t>fi</t>
+  </si>
+  <si>
+    <t>Proportion of dead biomass recycled to inert materials</t>
+  </si>
+  <si>
+    <t>µa</t>
+  </si>
+  <si>
+    <t>Specific growth rate of autotroph microorganisms</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>Nitrification</t>
+  </si>
+  <si>
+    <t>pmaxdenit</t>
+  </si>
+  <si>
+    <t>gN-(N2O+N2)g-1 NNO3 j-1</t>
+  </si>
+  <si>
+    <t>émission maximale de N2O et N2 à partir du NO3</t>
+  </si>
+  <si>
+    <t>ba</t>
+  </si>
+  <si>
+    <t>Vitesse de décès de la biomasse autotrophe</t>
+  </si>
+  <si>
+    <t>autotroph microorganisms</t>
+  </si>
+  <si>
+    <t>pdenit</t>
+  </si>
+  <si>
+    <t>gN2ON/g(N2O+N2)N</t>
+  </si>
+  <si>
+    <t>tiré de Oudart, moyenne des valeurs</t>
+  </si>
+  <si>
+    <t>https://composteur.online/taille-composteur/</t>
+  </si>
+  <si>
+    <t>Surface</t>
+  </si>
+  <si>
+    <t>En supposant des composteurs de 800 litres (3 à 4 pers)</t>
+  </si>
+  <si>
+    <t>https://www.suresnes.fr/wp-content/uploads/2019/05/fiche-technique-composteurs-bois-400-et-600-L.pdf</t>
+  </si>
+  <si>
+    <t>Dimensions (L*l*h)</t>
+  </si>
+  <si>
+    <t>1,010x1,010x1
+18mm épaisseur</t>
+  </si>
+  <si>
+    <t>HC wood</t>
+  </si>
+  <si>
+    <t>HC plastic</t>
+  </si>
+  <si>
+    <t>1W = 3,6 kJ/h</t>
+  </si>
+  <si>
+    <t>kJ/m2.°K.h</t>
+  </si>
+  <si>
+    <t>Bois</t>
+  </si>
+  <si>
+    <t>Polypropylène</t>
+  </si>
+  <si>
+    <t>Conductivités thermiques (W/mK)</t>
+  </si>
+  <si>
+    <t>hc wood</t>
+  </si>
+  <si>
+    <t>hc plastic</t>
+  </si>
+  <si>
+    <t>Pour 60 - 80 foyers</t>
+  </si>
+  <si>
+    <t>https://cdn.paris.fr/paris/2021/04/20/ddd25191c66e6da3abffd08d536d0fb1.pdf</t>
+  </si>
+  <si>
+    <t>1,5*1*0,8
+18 mm épaisseur</t>
+  </si>
+  <si>
+    <t>Industrial composting</t>
+  </si>
+  <si>
+    <t>H20</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>CH4</t>
+  </si>
+  <si>
+    <t>Methane from L</t>
+  </si>
+  <si>
+    <t>from HE</t>
+  </si>
+  <si>
+    <t>NH3</t>
+  </si>
+  <si>
+    <t>vmax</t>
+  </si>
+  <si>
+    <t>u*  (W/m2.K)</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>Capacités de déchets entrant</t>
+  </si>
+  <si>
+    <t>In vessel : Electromecanic</t>
+  </si>
 </sst>
 </file>
 
@@ -1388,7 +1540,7 @@
     <numFmt numFmtId="166" formatCode="0.000000"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1473,6 +1625,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1512,10 +1672,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1571,8 +1732,13 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1586,6 +1752,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>133068</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>244475</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>567</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01ECE040-D114-4771-8FA8-AB8D191A2AC4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11734800" y="675993"/>
+          <a:ext cx="4759325" cy="2982174"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>733424</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>35013</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{570B3267-94EF-43C6-BF26-D2360DB21770}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11687175" y="3740150"/>
+          <a:ext cx="4533899" cy="1762213"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1889,7 +2148,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H2" sqref="H2"/>
+      <selection pane="topRight" activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -25171,13 +25430,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35DF1B96-6F36-403A-A03F-B41BA123E54D}">
   <dimension ref="A1:CB97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="21.08984375" customWidth="1"/>
+    <col min="1" max="1" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.26953125" bestFit="1" customWidth="1"/>
     <col min="8" max="62" width="0" hidden="1" customWidth="1"/>
     <col min="65" max="65" width="0" hidden="1" customWidth="1"/>
     <col min="69" max="69" width="0" hidden="1" customWidth="1"/>
@@ -49214,10 +49474,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A13E0657-BE6C-45BC-B891-D54361BD0D37}">
-  <dimension ref="A1:M37"/>
+  <dimension ref="A1:S37"/>
   <sheetViews>
     <sheetView zoomScale="84" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -49230,7 +49490,7 @@
     <col min="12" max="12" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -49262,7 +49522,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>321</v>
       </c>
@@ -49295,8 +49555,17 @@
       <c r="M2">
         <v>0</v>
       </c>
+      <c r="Q2" t="s">
+        <v>489</v>
+      </c>
+      <c r="R2" t="s">
+        <v>490</v>
+      </c>
+      <c r="S2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -49332,8 +49601,23 @@
       <c r="M3">
         <v>1</v>
       </c>
+      <c r="P3" t="s">
+        <v>486</v>
+      </c>
+      <c r="Q3">
+        <f>(F4-(G4/4)-(H4/2))</f>
+        <v>12.25</v>
+      </c>
+      <c r="R3">
+        <f>F5-(G5/4)-(H5/2)</f>
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <f>(F3-(G3/4)-(H3/2)+((3*I3)/4))</f>
+        <v>10.5</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -49366,8 +49650,23 @@
       <c r="M4">
         <v>2</v>
       </c>
+      <c r="P4" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q4">
+        <f>(F4/2)-(G4/8)+(H4/4)</f>
+        <v>7.625</v>
+      </c>
+      <c r="R4">
+        <f>(F5/2)-(G5/8)+(H5/4)</f>
+        <v>5</v>
+      </c>
+      <c r="S4">
+        <f>(F3/2)-(G3/8)+(H3/4)+((3*I3)/8)</f>
+        <v>7.75</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>322</v>
       </c>
@@ -49400,8 +49699,23 @@
       <c r="M5">
         <v>3</v>
       </c>
+      <c r="P5" t="s">
+        <v>488</v>
+      </c>
+      <c r="Q5">
+        <f>(F4/2)+(G4/8)-(H4/4)</f>
+        <v>17.375</v>
+      </c>
+      <c r="R5">
+        <f>(F6/2)+(G6/8)-(H6/4)</f>
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <f>(F3/2)+(G3/8)-(H3/4)-((3*I3)/8)</f>
+        <v>8.25</v>
+      </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -49425,8 +49739,15 @@
       <c r="M6">
         <v>4</v>
       </c>
+      <c r="P6" t="s">
+        <v>491</v>
+      </c>
+      <c r="S6">
+        <f>I3</f>
+        <v>4</v>
+      </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
@@ -49460,7 +49781,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>295</v>
       </c>
@@ -49481,7 +49802,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -49514,7 +49835,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -49550,7 +49871,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -49583,7 +49904,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -49613,7 +49934,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -49646,7 +49967,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -49682,7 +50003,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>29</v>
       </c>
@@ -49718,7 +50039,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>31</v>
       </c>
@@ -49869,8 +50190,12 @@
       <c r="B20">
         <v>0.1</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+      <c r="C20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>463</v>
+      </c>
       <c r="E20" s="2" t="s">
         <v>323</v>
       </c>
@@ -49954,6 +50279,9 @@
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>400</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>6</v>
@@ -50106,10 +50434,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02BDDFCB-2B9F-4872-A820-97635CABD872}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -50117,7 +50445,7 @@
     <col min="1" max="1" width="8.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>407</v>
       </c>
@@ -50125,7 +50453,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>409</v>
       </c>
@@ -50133,7 +50461,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>325</v>
       </c>
@@ -50142,7 +50470,7 @@
         <v>0.55752212389380529</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>326</v>
       </c>
@@ -50151,7 +50479,7 @@
         <v>1.0902654867256636</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>327</v>
       </c>
@@ -50160,7 +50488,7 @@
         <v>1.2172566371681415</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>328</v>
       </c>
@@ -50169,7 +50497,7 @@
         <v>0.42743362831858406</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>329</v>
       </c>
@@ -50178,7 +50506,7 @@
         <v>0.25506072874493924</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>330</v>
       </c>
@@ -50187,7 +50515,7 @@
         <v>0.49878542510121454</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>331</v>
       </c>
@@ -50196,7 +50524,7 @@
         <v>0.55688259109311733</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>332</v>
       </c>
@@ -50205,7 +50533,7 @@
         <v>0.19554655870445342</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>333</v>
       </c>
@@ -50214,12 +50542,63 @@
         <v>0.51862348178137652</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>405</v>
       </c>
       <c r="B12" s="2">
         <v>0.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="B13">
+        <v>1.83</v>
+      </c>
+      <c r="C13" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="B14">
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="B15">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="B16">
+        <v>1.0409999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="B17">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="B18">
+        <v>1.88</v>
       </c>
     </row>
   </sheetData>
@@ -50230,17 +50609,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99E22A85-0A6D-4692-91B9-50CA4D04329A}">
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.6328125" style="23" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.6328125" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.36328125" style="23" customWidth="1"/>
     <col min="4" max="4" width="45.54296875" style="23" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="10.90625" style="23"/>
   </cols>
@@ -50823,7 +51202,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
-        <v>338</v>
+        <v>446</v>
       </c>
       <c r="B36" s="2">
         <v>57.2</v>
@@ -50837,7 +51216,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
-        <v>334</v>
+        <v>445</v>
       </c>
       <c r="B37" s="2">
         <v>65.5</v>
@@ -50961,115 +51340,188 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="23" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B46" s="23">
         <v>404</v>
       </c>
       <c r="C46" s="23" t="s">
+        <v>422</v>
+      </c>
+      <c r="D46" s="23" t="s">
+        <v>423</v>
+      </c>
+      <c r="E46" s="23" t="s">
         <v>424</v>
-      </c>
-      <c r="D46" s="23" t="s">
-        <v>425</v>
-      </c>
-      <c r="E46" s="23" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="23" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B47" s="23">
         <v>1005</v>
       </c>
       <c r="C47" s="23" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D47" s="23" t="s">
+        <v>426</v>
+      </c>
+      <c r="E47" s="23" t="s">
         <v>428</v>
-      </c>
-      <c r="E47" s="23" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="23" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B48" s="23">
         <v>710</v>
       </c>
       <c r="C48" s="23" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D48" s="23" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="E48" s="23" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="F48" s="23" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="23" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B49" s="26">
         <v>1000</v>
       </c>
       <c r="C49" s="26" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="23" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B50" s="30">
         <v>1260</v>
       </c>
       <c r="C50" s="23" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D50" s="23" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E50" s="23" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="23" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B51" s="23">
         <v>1542</v>
       </c>
       <c r="C51" s="23" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D51" s="23" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="E51" s="23" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="23" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B52" s="23">
         <v>1305</v>
       </c>
       <c r="C52" s="23" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E52" s="23" t="s">
-        <v>442</v>
+        <v>440</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" s="27" t="s">
+        <v>447</v>
+      </c>
+      <c r="B53" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="C53"/>
+      <c r="D53" s="2" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" s="23" t="s">
+        <v>449</v>
+      </c>
+      <c r="B54" s="23">
+        <v>0.03</v>
+      </c>
+      <c r="C54" s="23" t="s">
+        <v>257</v>
+      </c>
+      <c r="D54" s="23" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" s="27" t="s">
+        <v>458</v>
+      </c>
+      <c r="B55" s="27">
+        <v>1</v>
+      </c>
+      <c r="C55" s="27" t="s">
+        <v>459</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="B56" s="2">
+        <v>8.3000000000000001E-3</v>
+      </c>
+      <c r="C56" s="23" t="s">
+        <v>257</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" s="26" t="s">
+        <v>464</v>
+      </c>
+      <c r="B57" s="26">
+        <v>0.125</v>
+      </c>
+      <c r="C57" s="26" t="s">
+        <v>465</v>
+      </c>
+      <c r="D57" s="27" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A58" s="23" t="s">
+        <v>492</v>
       </c>
     </row>
   </sheetData>
@@ -51080,124 +51532,241 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68CD580C-396B-4BB3-AD93-6F2493BB33D0}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="5" max="5" width="9.453125" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" customWidth="1"/>
+    <col min="5" max="5" width="20.453125" customWidth="1"/>
     <col min="6" max="6" width="13.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="J1" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="B2" s="2">
+        <f>(D10*3.6)</f>
+        <v>240.00000000000003</v>
+      </c>
+      <c r="C2" s="2">
+        <f>(1.01*1*4)+(1.01*1.01)</f>
+        <v>5.0601000000000003</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>475</v>
+      </c>
+      <c r="J2" t="s">
+        <v>477</v>
+      </c>
+      <c r="K2">
+        <v>0.12</v>
+      </c>
+      <c r="N2" s="32" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="B3" s="2">
+        <f>D11*3.6</f>
+        <v>400</v>
+      </c>
+      <c r="C3" s="2">
+        <f>(1.01*1*4)+(1.01*1.01)</f>
+        <v>5.0601000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="B4" s="2">
+        <f>D12*3.6</f>
+        <v>240.00000000000003</v>
+      </c>
+      <c r="C4">
+        <f>(1.5*0.8*3)+(1.5*1)</f>
+        <v>5.1000000000000005</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="J4" t="s">
+        <v>478</v>
+      </c>
+      <c r="K4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="B5" s="2">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>431</v>
+      <c r="D7" s="2" t="s">
+        <v>430</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="B2" s="2">
-        <v>12</v>
-      </c>
-      <c r="C2" s="2">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="B3" s="2">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2">
-        <v>4</v>
-      </c>
-      <c r="D3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="B4" s="2">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2">
-        <v>15</v>
-      </c>
-      <c r="D4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="D9" t="s">
+        <v>493</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>494</v>
+      </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+    <row r="10" spans="1:14" ht="24.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>472</v>
+      </c>
+      <c r="C10" s="2">
+        <f>(1.01*1*4)+(1.01*1.01)</f>
+        <v>5.0601000000000003</v>
+      </c>
+      <c r="D10">
+        <f>(1/(0.0018/0.12))</f>
+        <v>66.666666666666671</v>
+      </c>
+      <c r="F10" t="s">
+        <v>469</v>
+      </c>
+      <c r="G10" s="32" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="24.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>472</v>
+      </c>
+      <c r="C11" s="2">
+        <f>(1.01*1*4)+(1.01*1.01)</f>
+        <v>5.0601000000000003</v>
+      </c>
+      <c r="D11">
+        <f>1/(0.0018/0.2)</f>
+        <v>111.11111111111111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="24.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>484</v>
+      </c>
+      <c r="C12">
+        <f>(1.5*0.8*3)+(1.5*1)</f>
+        <v>5.1000000000000005</v>
+      </c>
+      <c r="D12">
+        <f>(1/(0.0018/0.12))</f>
+        <v>66.666666666666671</v>
+      </c>
+      <c r="F12" t="s">
+        <v>482</v>
+      </c>
+      <c r="G12" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>496</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G10" r:id="rId1" xr:uid="{1CEABAA3-6617-4EB3-9F2D-C93F4943CEA5}"/>
+    <hyperlink ref="N2" r:id="rId2" xr:uid="{6C69F668-A99C-45F7-9F36-6842FD76DCAE}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="597" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="597" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -51218,7 +51787,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B2">
         <v>20</v>

</xml_diff>